<commit_message>
Atualizando documento de transacoes
</commit_message>
<xml_diff>
--- a/documentos/SLOL-Transacoes.xlsx
+++ b/documentos/SLOL-Transacoes.xlsx
@@ -182,7 +182,8 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <rFont val="Arial"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -271,7 +272,8 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <rFont val="Arial"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -459,7 +461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t xml:space="preserve">Manutenção de Cadastros</t>
   </si>
@@ -513,6 +515,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reserva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrar</t>
   </si>
   <si>
     <t xml:space="preserve">Relatórios</t>
@@ -553,7 +558,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -589,12 +594,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -774,10 +773,10 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.99"/>
@@ -1092,7 +1091,9 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1153,7 +1154,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1172,28 +1173,28 @@
         <v>2</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J23" s="2"/>
     </row>
@@ -1278,7 +1279,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="6" t="n">
         <f aca="false">J3+J16+J24</f>
@@ -1319,7 +1320,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1342,7 +1343,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>